<commit_message>
Updates after running trials on final product
</commit_message>
<xml_diff>
--- a/Database/USER_DATABASE.xlsx
+++ b/Database/USER_DATABASE.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>First Name</t>
   </si>
@@ -28,34 +28,10 @@
     <t>Weight After Workout (lbs)</t>
   </si>
   <si>
-    <t>Jason</t>
-  </si>
-  <si>
-    <t>Morgan</t>
-  </si>
-  <si>
-    <t>Ray</t>
-  </si>
-  <si>
-    <t>Vu</t>
-  </si>
-  <si>
-    <t>Th</t>
-  </si>
-  <si>
-    <t>Profancik</t>
-  </si>
-  <si>
-    <t>Downing</t>
-  </si>
-  <si>
-    <t>Doromal</t>
-  </si>
-  <si>
-    <t>Dinh</t>
-  </si>
-  <si>
-    <t>Yu</t>
+    <t>Dispenser</t>
+  </si>
+  <si>
+    <t>Water</t>
   </si>
 </sst>
 </file>
@@ -413,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,69 +414,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>190</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>190</v>
-      </c>
-      <c r="D4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>500</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>11236</v>
-      </c>
-      <c r="D6">
-        <v>522</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>